<commit_message>
All models now work.
</commit_message>
<xml_diff>
--- a/Projects/VoortoetsAGT/cases/Generic/Generic.xlsx
+++ b/Projects/VoortoetsAGT/cases/Generic/Generic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/Generic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE53841A-9F5C-A74A-A3D8-86251CA372AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72FEEAF-6B22-8240-A44E-E307CCEA8C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="-26760" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11860" yWindow="-26760" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -11910,10 +11910,13 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">

</xml_diff>

<commit_message>
Two cases added to mf6lab under Compare_fdm3t, which compares Modflow with ffdm3t and analytic approach for Hantus and Bruggeman 220_03.
</commit_message>
<xml_diff>
--- a/Projects/VoortoetsAGT/cases/Generic/Generic.xlsx
+++ b/Projects/VoortoetsAGT/cases/Generic/Generic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/Generic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28F7B0E-8075-D941-BE33-1E11AD86729D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5A7DA6-4CFF-9B45-8EA5-2FF531E0DF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="-26760" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -1669,9 +1669,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1709,7 +1709,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1815,7 +1815,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1957,7 +1957,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1967,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3543,7 +3543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A408" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+    <sheetView topLeftCell="A463" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
       <selection activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
@@ -11837,8 +11837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11888,13 +11888,13 @@
         <v>10958</v>
       </c>
       <c r="D3" s="10">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E3" s="10">
         <v>1.25</v>
       </c>
       <c r="F3" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>